<commit_message>
adapted tests for SQLSource
</commit_message>
<xml_diff>
--- a/TableReaderTest/ForSourceTest/TextSample.xlsx
+++ b/TableReaderTest/ForSourceTest/TextSample.xlsx
@@ -19,21 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>col0</t>
-  </si>
-  <si>
-    <t>col1</t>
-  </si>
-  <si>
-    <t>col2</t>
-  </si>
-  <si>
-    <t>col3</t>
-  </si>
-  <si>
-    <t>col4</t>
   </si>
   <si>
     <t>Рус</t>
@@ -43,6 +31,9 @@
   </si>
   <si>
     <t>1 2</t>
+  </si>
+  <si>
+    <t>11:11:11</t>
   </si>
 </sst>
 </file>
@@ -544,12 +535,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -874,7 +866,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -890,22 +882,20 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="4">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>34.4</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4">
         <v>25</v>
@@ -922,7 +912,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -939,7 +929,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4">
         <v>-10</v>

</xml_diff>